<commit_message>
update tableau et stage 2
</commit_message>
<xml_diff>
--- a/images/E4.xlsx
+++ b/images/E4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marie\Desktop\portfolio\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57B0747F-4C81-4BB4-82B5-63E79DF3A9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF101E84-6D4F-43FF-9485-CFD658243E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -117,9 +117,6 @@
     <t>SESSION 2022</t>
   </si>
   <si>
-    <t xml:space="preserve">N° candidat : </t>
-  </si>
-  <si>
     <t>Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
   </si>
   <si>
@@ -132,15 +129,9 @@
     <t>NOM et prénom :  UCLES MARIE</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio : https://github.com/Mariecls/Portfolio-Marie-</t>
-  </si>
-  <si>
     <t>Centre de formation : Lycée Charles de Foucauld, Paris 18ème</t>
   </si>
   <si>
-    <t xml:space="preserve">Projet  Parking itération 1 , gérant l'attributions de place de parking avec un MCD, documentation et maquettes </t>
-  </si>
-  <si>
     <t>Projet Festival Sp'Or Hébergement des Groupes , gérant l'hébergement des ligues de sport durant le festival Sp'Or suivant le modèle MVC en php  avec code en php  et compte rendu</t>
   </si>
   <si>
@@ -159,15 +150,9 @@
     <t>Création de mon CV en html/CSS</t>
   </si>
   <si>
-    <t>Mise en place d'une veille</t>
-  </si>
-  <si>
     <t>du 9/05/2022  au 10/06/2022</t>
   </si>
   <si>
-    <t>du 3/01/2022 au 3/02/2022</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -186,15 +171,9 @@
     <t>du 20/04/2022 au 12/12/2022</t>
   </si>
   <si>
-    <t xml:space="preserve">Projet Boite à idées , forum avec création d' idées sur les erreurs de l'application </t>
-  </si>
-  <si>
     <t>du 5/12/2022 au 12/12/2022</t>
   </si>
   <si>
-    <t>du 14/11/2022 au 14/11/2022</t>
-  </si>
-  <si>
     <t>du 08/09/2021 au 12/11/2022</t>
   </si>
   <si>
@@ -207,26 +186,10 @@
     <t>du 12/11/2021 au 10/12/2021</t>
   </si>
   <si>
-    <t xml:space="preserve">TP Devis </t>
-  </si>
-  <si>
     <t>du 7/10/2021 au 21/12/2021</t>
   </si>
   <si>
     <t xml:space="preserve">Site web BMA création de pages en HTML CSS et site lancé après la fin du stage </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Partcipation à une réunion avant la mise en place du site web de AAMTC et choix de l'image d'accueil afin de faire valider par l'entreprise par la suite</t>
-    </r>
   </si>
   <si>
     <r>
@@ -256,6 +219,33 @@
   <si>
     <t xml:space="preserve">Amélioration du site fiertile et mise en place d'une fiche sur les points à améliorer sur chaque page pour améliorer le référencement et exéprience client </t>
   </si>
+  <si>
+    <t>du 15/11/2022 au 29/03/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projet  Parking  , gérant l'attributions de place de parking avec un MCD, documentation et maquettes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en place d'une veille et portfolio </t>
+  </si>
+  <si>
+    <t>TP STARTUP, création d'une start-up fictive</t>
+  </si>
+  <si>
+    <t>TP Devis,création d'un devis de proposition de matériel informatique</t>
+  </si>
+  <si>
+    <t>du 3/01/2023 au 3/02/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participation au projet Anyway , programmation en PHP sous Laravel </t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://mariecls.github.io/Portfolio-Marie-/</t>
+  </si>
+  <si>
+    <t>N° candidat : 02243902313</t>
+  </si>
 </sst>
 </file>
 
@@ -264,7 +254,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -337,6 +327,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -346,7 +342,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -451,51 +447,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
     <border diagonalDown="1">
       <left style="medium">
         <color theme="2" tint="-0.749992370372631"/>
@@ -737,7 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -760,17 +711,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -784,100 +729,94 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -896,6 +835,111 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Connecteur droit 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57E9A2C0-6C29-5746-C73F-F0E8ED979B2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18945225" y="1743075"/>
+          <a:ext cx="133350" cy="76200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connecteur droit 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDD1EC40-AF40-DE97-D3C1-EF8D050FFCB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="18964275" y="1724025"/>
+          <a:ext cx="152400" cy="104775"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1222,10 +1266,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ83"/>
+  <dimension ref="A1:AQ76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1238,84 +1282,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="20"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="28"/>
+      <c r="A3" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="36"/>
+      <c r="H3" s="42"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="12" t="s">
+      <c r="A4" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
+      <c r="A5" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>21</v>
+      <c r="B6" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>0</v>
@@ -1337,8 +1381,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
-      <c r="B7" s="38"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1394,16 +1438,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="33"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1441,24 +1485,24 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="47"/>
+      <c r="A9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="20"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1496,20 +1540,24 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="47"/>
+      <c r="A10" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="20"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1547,24 +1595,24 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="47"/>
+      <c r="A11" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="20"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1602,24 +1650,22 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="47"/>
+      <c r="A12" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="20"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1657,22 +1703,22 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="47"/>
+      <c r="A13" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="20"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1710,22 +1756,22 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="44" t="s">
+      <c r="A14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="47"/>
+      <c r="D14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="20"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1763,22 +1809,22 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14" t="s">
+      <c r="A15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="47"/>
+      <c r="C15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="20"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1816,19 +1862,19 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="47" t="s">
-        <v>37</v>
+      <c r="A16" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="I16"/>
       <c r="J16"/>
@@ -1867,19 +1913,19 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="47" t="s">
-        <v>37</v>
+      <c r="A17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -1918,19 +1964,19 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="47" t="s">
-        <v>37</v>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="I18"/>
       <c r="J18"/>
@@ -1969,19 +2015,19 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="47" t="s">
-        <v>37</v>
+      <c r="A19" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
@@ -2020,16 +2066,16 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="36"/>
+      <c r="A20" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="29"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -2067,19 +2113,21 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="47" t="s">
-        <v>37</v>
+      <c r="A21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="I21"/>
       <c r="J21"/>
@@ -2118,26 +2166,26 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22" s="47"/>
+      <c r="A22" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="20"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2175,26 +2223,26 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23" s="47"/>
+      <c r="A23" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="H23" s="20"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2232,24 +2280,26 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="47"/>
+      <c r="A24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="20"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2287,24 +2337,22 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="47"/>
+      <c r="A25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="12"/>
+      <c r="H25" s="20"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2342,20 +2390,26 @@
       <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="47"/>
+      <c r="A26" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="20"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2393,24 +2447,22 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="47"/>
+      <c r="A27" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="12"/>
+      <c r="H27" s="20"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2447,21 +2499,17 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="47"/>
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="29"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2498,17 +2546,25 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="36"/>
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="43"/>
+      <c r="F29" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="14"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2545,17 +2601,15 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="16"/>
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2592,344 +2646,24 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="16"/>
-      <c r="I31"/>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-      <c r="N31"/>
-      <c r="O31"/>
-      <c r="P31"/>
-      <c r="Q31"/>
-      <c r="R31"/>
-      <c r="S31"/>
-      <c r="T31"/>
-      <c r="U31"/>
-      <c r="V31"/>
-      <c r="W31"/>
-      <c r="X31"/>
-      <c r="Y31"/>
-      <c r="Z31"/>
-      <c r="AA31"/>
-      <c r="AB31"/>
-      <c r="AC31"/>
-      <c r="AD31"/>
-      <c r="AE31"/>
-      <c r="AF31"/>
-      <c r="AG31"/>
-      <c r="AH31"/>
-      <c r="AI31"/>
-      <c r="AJ31"/>
-      <c r="AK31"/>
-      <c r="AL31"/>
-      <c r="AM31"/>
-      <c r="AN31"/>
-      <c r="AO31"/>
-      <c r="AP31"/>
-      <c r="AQ31"/>
-    </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="16"/>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32"/>
-      <c r="S32"/>
-      <c r="T32"/>
-      <c r="U32"/>
-      <c r="V32"/>
-      <c r="W32"/>
-      <c r="X32"/>
-      <c r="Y32"/>
-      <c r="Z32"/>
-      <c r="AA32"/>
-      <c r="AB32"/>
-      <c r="AC32"/>
-      <c r="AD32"/>
-      <c r="AE32"/>
-      <c r="AF32"/>
-      <c r="AG32"/>
-      <c r="AH32"/>
-      <c r="AI32"/>
-      <c r="AJ32"/>
-      <c r="AK32"/>
-      <c r="AL32"/>
-      <c r="AM32"/>
-      <c r="AN32"/>
-      <c r="AO32"/>
-      <c r="AP32"/>
-      <c r="AQ32"/>
-    </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="16"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-      <c r="N33"/>
-      <c r="O33"/>
-      <c r="P33"/>
-      <c r="Q33"/>
-      <c r="R33"/>
-      <c r="S33"/>
-      <c r="T33"/>
-      <c r="U33"/>
-      <c r="V33"/>
-      <c r="W33"/>
-      <c r="X33"/>
-      <c r="Y33"/>
-      <c r="Z33"/>
-      <c r="AA33"/>
-      <c r="AB33"/>
-      <c r="AC33"/>
-      <c r="AD33"/>
-      <c r="AE33"/>
-      <c r="AF33"/>
-      <c r="AG33"/>
-      <c r="AH33"/>
-      <c r="AI33"/>
-      <c r="AJ33"/>
-      <c r="AK33"/>
-      <c r="AL33"/>
-      <c r="AM33"/>
-      <c r="AN33"/>
-      <c r="AO33"/>
-      <c r="AP33"/>
-      <c r="AQ33"/>
-    </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="16"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34"/>
-      <c r="P34"/>
-      <c r="Q34"/>
-      <c r="R34"/>
-      <c r="S34"/>
-      <c r="T34"/>
-      <c r="U34"/>
-      <c r="V34"/>
-      <c r="W34"/>
-      <c r="X34"/>
-      <c r="Y34"/>
-      <c r="Z34"/>
-      <c r="AA34"/>
-      <c r="AB34"/>
-      <c r="AC34"/>
-      <c r="AD34"/>
-      <c r="AE34"/>
-      <c r="AF34"/>
-      <c r="AG34"/>
-      <c r="AH34"/>
-      <c r="AI34"/>
-      <c r="AJ34"/>
-      <c r="AK34"/>
-      <c r="AL34"/>
-      <c r="AM34"/>
-      <c r="AN34"/>
-      <c r="AO34"/>
-      <c r="AP34"/>
-      <c r="AQ34"/>
-    </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="16"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
-      <c r="AF35"/>
-      <c r="AG35"/>
-      <c r="AH35"/>
-      <c r="AI35"/>
-      <c r="AJ35"/>
-      <c r="AK35"/>
-      <c r="AL35"/>
-      <c r="AM35"/>
-      <c r="AN35"/>
-      <c r="AO35"/>
-      <c r="AP35"/>
-      <c r="AQ35"/>
-    </row>
-    <row r="36" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="18"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="R36"/>
-      <c r="S36"/>
-      <c r="T36"/>
-      <c r="U36"/>
-      <c r="V36"/>
-      <c r="W36"/>
-      <c r="X36"/>
-      <c r="Y36"/>
-      <c r="Z36"/>
-      <c r="AA36"/>
-      <c r="AB36"/>
-      <c r="AC36"/>
-      <c r="AD36"/>
-      <c r="AE36"/>
-      <c r="AF36"/>
-      <c r="AG36"/>
-      <c r="AH36"/>
-      <c r="AI36"/>
-      <c r="AJ36"/>
-      <c r="AK36"/>
-      <c r="AL36"/>
-      <c r="AM36"/>
-      <c r="AN36"/>
-      <c r="AO36"/>
-      <c r="AP36"/>
-      <c r="AQ36"/>
-    </row>
-    <row r="37" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37"/>
-      <c r="M37"/>
-      <c r="N37"/>
-      <c r="O37"/>
-      <c r="P37"/>
-      <c r="Q37"/>
-      <c r="R37"/>
-      <c r="S37"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-      <c r="X37"/>
-      <c r="Y37"/>
-      <c r="Z37"/>
-      <c r="AA37"/>
-      <c r="AB37"/>
-      <c r="AC37"/>
-      <c r="AD37"/>
-      <c r="AE37"/>
-      <c r="AF37"/>
-      <c r="AG37"/>
-      <c r="AH37"/>
-      <c r="AI37"/>
-      <c r="AJ37"/>
-      <c r="AK37"/>
-      <c r="AL37"/>
-      <c r="AM37"/>
-      <c r="AN37"/>
-      <c r="AO37"/>
-      <c r="AP37"/>
-      <c r="AQ37"/>
-    </row>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2958,32 +2692,26 @@
     <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A5:H5"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A5:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="48" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>